<commit_message>
- Penambahan user superadmin - Penambahan fitur Templates
</commit_message>
<xml_diff>
--- a/storage/app/public/files/Report_Call_Logs.xlsx
+++ b/storage/app/public/files/Report_Call_Logs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\XAMPP\xampp5\htdocs\ivr-blast\storage\app\public\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\htdocs\ivrblast\storage\app\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A962FEFD-D0BE-491D-BD05-F7675EA55790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73DD8E47-F273-4740-95D0-118F2D3198B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{494AA093-F60E-40B8-A3BD-38F34CC74876}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{494AA093-F60E-40B8-A3BD-38F34CC74876}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,49 +25,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>ACCOUNT_ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>Report Call Logs</t>
   </si>
-  <si>
-    <t>CALL_DATE</t>
-  </si>
-  <si>
-    <t>PHONE NUMBER</t>
-  </si>
-  <si>
-    <t>DIAL</t>
-  </si>
-  <si>
-    <t>CONNECT</t>
-  </si>
-  <si>
-    <t>DISCONNECT</t>
-  </si>
-  <si>
-    <t>DURATION</t>
-  </si>
-  <si>
-    <t>CALL RESPONSE</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -91,7 +59,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -99,34 +67,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAAAF970-3DE8-437C-BC97-5CD527F67FF0}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -464,7 +413,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -474,46 +423,9 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>